<commit_message>
from-7th-commit with drag and drop-1
</commit_message>
<xml_diff>
--- a/backend/media/update/.xlsx
+++ b/backend/media/update/.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,38 +444,60 @@
           <t>required</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>appearance</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>parameters</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>select_one zEdBNsf</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>what_is_your_name?</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Choiice</t>
+          <t>What is your name?</t>
         </is>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>what_is_your_age?</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>What is your age?</t>
         </is>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -506,7 +528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,32 +553,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>zEdBNsf</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>option_1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>zEdBNsf</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>option_2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
from-8th-commit with from segmentatioin
</commit_message>
<xml_diff>
--- a/backend/media/update/.xlsx
+++ b/backend/media/update/.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,21 +454,41 @@
           <t>parameters</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>hint</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>default</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>guidance_hint</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>hxl</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>image</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>what_is_your_name?</t>
+          <t>this_is_image</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What is your name?</t>
+          <t>This is image</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -476,28 +496,10 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>integer</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>what_is_your_age?</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>What is your age?</t>
-        </is>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>